<commit_message>
Update figure 3️⃣ code for publication
Adding analysis code for the euclidean distance measurments in colabfold predicted pdb models
</commit_message>
<xml_diff>
--- a/_Code/Fig3/tables/Gradient_WB_quantifications.xlsx
+++ b/_Code/Fig3/tables/Gradient_WB_quantifications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://crgcnag-my.sharepoint.com/personal/narecco_crg_es/Documents/Suz12_AS_project/_Code/Fig3/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="14_{E21DE725-0EC2-8A45-B1AA-0B985B8BF59D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{97EAF340-8DB5-6B46-9D50-69EBB1C20C0A}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="14_{E21DE725-0EC2-8A45-B1AA-0B985B8BF59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9D5EF49-8446-964E-AECC-E0EA681A298B}"/>
   <bookViews>
-    <workbookView xWindow="-57660" yWindow="460" windowWidth="19240" windowHeight="11440" activeTab="4" xr2:uid="{815DCC61-5122-5648-BAF8-251F2ADD42C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" activeTab="1" xr2:uid="{815DCC61-5122-5648-BAF8-251F2ADD42C7}"/>
   </bookViews>
   <sheets>
     <sheet name="WT_1" sheetId="1" r:id="rId1"/>
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B6ADB9-484E-EE44-8630-B51B37E65990}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E21:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>659722</v>
+        <v>24102</v>
       </c>
       <c r="C2">
         <v>65896</v>
@@ -821,7 +821,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>483823</v>
+        <v>34545</v>
       </c>
       <c r="C3">
         <v>322294</v>
@@ -844,7 +844,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>586076</v>
+        <v>658817</v>
       </c>
       <c r="C4">
         <v>195550</v>
@@ -867,7 +867,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>2843908</v>
+        <v>10613437</v>
       </c>
       <c r="C5">
         <v>311799</v>
@@ -890,7 +890,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>2582406</v>
+        <v>7169087</v>
       </c>
       <c r="C6">
         <v>204148</v>
@@ -913,7 +913,7 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>2362171</v>
+        <v>5161263</v>
       </c>
       <c r="C7">
         <v>1161788</v>
@@ -936,7 +936,7 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>2855204</v>
+        <v>7985127</v>
       </c>
       <c r="C8">
         <v>4537874</v>
@@ -959,7 +959,7 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>2915010</v>
+        <v>7405939</v>
       </c>
       <c r="C9">
         <v>7777363</v>
@@ -982,7 +982,7 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>510199</v>
+        <v>1476866</v>
       </c>
       <c r="C10">
         <v>1431045</v>
@@ -1005,7 +1005,7 @@
         <v>20</v>
       </c>
       <c r="B11">
-        <v>417199</v>
+        <v>557280</v>
       </c>
       <c r="C11">
         <v>692132</v>
@@ -1028,7 +1028,7 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <v>304595</v>
+        <v>70910</v>
       </c>
       <c r="C12">
         <v>147818</v>
@@ -1051,7 +1051,7 @@
         <v>24</v>
       </c>
       <c r="B13">
-        <v>367599</v>
+        <v>28789</v>
       </c>
       <c r="C13">
         <v>102064</v>
@@ -1859,7 +1859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035BD968-DF2C-544A-B49A-79D9E08FB9E8}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>

</xml_diff>